<commit_message>
alter the normal rule of disturbance
</commit_message>
<xml_diff>
--- a/output/experiments/thesis_topic1/6h-bat-12month-0.6dc.xlsx
+++ b/output/experiments/thesis_topic1/6h-bat-12month-0.6dc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\Coding_project\Energy_grid_new\output\experiments\thesis_topic1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD67946-002C-458C-8ABB-8CA5784D7709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5B3659-2410-4743-A4CF-BAEB8B0CDE1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="83">
   <si>
     <t>status</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>month_of_year</t>
+  </si>
+  <si>
+    <t>disturbance_scale</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:BC73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -750,7 +753,7 @@
         <v>68</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>16</v>

</xml_diff>